<commit_message>
final excel - name + PN + Abrk
</commit_message>
<xml_diff>
--- a/Qualität_12_24.xlsx
+++ b/Qualität_12_24.xlsx
@@ -504,7 +504,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Pan pes</t>
+          <t>1002000/44444/Pan pes</t>
         </is>
       </c>
       <c r="O2" t="n">
@@ -514,7 +514,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Pan les</t>
+          <t>None/None/Pan les</t>
         </is>
       </c>
       <c r="O3" t="n">

</xml_diff>

<commit_message>
Month count shown in final excel
</commit_message>
<xml_diff>
--- a/Qualität_12_24.xlsx
+++ b/Qualität_12_24.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,6 +507,9 @@
           <t>1002000/44444/Pan pes</t>
         </is>
       </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
       <c r="O2" t="n">
         <v>30</v>
       </c>
@@ -517,8 +520,22 @@
           <t>None/None/Pan les</t>
         </is>
       </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
       <c r="O3" t="n">
         <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>